<commit_message>
Remove large files from repo history, I believe
</commit_message>
<xml_diff>
--- a/scrape_mountain_weather_data/analysis/avg_morning_chill_june_2024_excel.xlsx
+++ b/scrape_mountain_weather_data/analysis/avg_morning_chill_june_2024_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd862b9fb7d60430/Desktop/repos/scrape-mountain-weather-data/scrape_mountain_weather_data/data/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmwad\OneDrive\Desktop\repos\scrape-mountain-weather-data\scrape_mountain_weather_data\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{5E9817B7-6841-4FE4-97CA-9B9436596081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2E1557A-2375-4776-986A-A252BEE6C7FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0097DAAE-329A-49D4-9035-4CD59BD77114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A48DE54E-D8C0-4CF6-92BB-8002D761C2DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{A48DE54E-D8C0-4CF6-92BB-8002D761C2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="chill vs elevation, karakoram" sheetId="3" r:id="rId3"/>
     <sheet name="chill at 4-4500m vs. abs. lat" sheetId="5" r:id="rId4"/>
     <sheet name="chill vs. avg. windspeed" sheetId="6" r:id="rId5"/>
+    <sheet name="data for 3d plot" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="79">
   <si>
     <t>mtn_name</t>
   </si>
@@ -4156,7 +4157,7 @@
   <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9825,7 +9826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BE5266-FC73-4D9D-9C49-A5AB744C0DAF}">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -11225,4 +11226,2547 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CD232B-E5ED-49DF-9162-19843A25CEDF}">
+  <dimension ref="A1:F126"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>45.832500000000003</v>
+      </c>
+      <c r="C2">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="D2">
+        <v>3000</v>
+      </c>
+      <c r="E2">
+        <v>-0.32</v>
+      </c>
+      <c r="F2">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>45.832500000000003</v>
+      </c>
+      <c r="C3">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="D3">
+        <v>4807</v>
+      </c>
+      <c r="E3">
+        <v>-18.21</v>
+      </c>
+      <c r="F3">
+        <v>31.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>45.832500000000003</v>
+      </c>
+      <c r="C4">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>14.35</v>
+      </c>
+      <c r="F4">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>45.832500000000003</v>
+      </c>
+      <c r="C5">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5">
+        <v>7.38</v>
+      </c>
+      <c r="F5">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>45.832500000000003</v>
+      </c>
+      <c r="C6">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="D6">
+        <v>4000</v>
+      </c>
+      <c r="E6">
+        <v>-10.32</v>
+      </c>
+      <c r="F6">
+        <v>21.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>44.27</v>
+      </c>
+      <c r="C7">
+        <v>71.303060000000002</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>12.85</v>
+      </c>
+      <c r="F7">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>44.27</v>
+      </c>
+      <c r="C8">
+        <v>71.303060000000002</v>
+      </c>
+      <c r="D8">
+        <v>1917</v>
+      </c>
+      <c r="E8">
+        <v>5.56</v>
+      </c>
+      <c r="F8">
+        <v>25.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>35.765000000000001</v>
+      </c>
+      <c r="C9">
+        <v>82.265280000000004</v>
+      </c>
+      <c r="D9">
+        <v>1500</v>
+      </c>
+      <c r="E9">
+        <v>15.18</v>
+      </c>
+      <c r="F9">
+        <v>11.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>35.765000000000001</v>
+      </c>
+      <c r="C10">
+        <v>82.265280000000004</v>
+      </c>
+      <c r="D10">
+        <v>2037</v>
+      </c>
+      <c r="E10">
+        <v>11.82</v>
+      </c>
+      <c r="F10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>35.765000000000001</v>
+      </c>
+      <c r="C11">
+        <v>82.265280000000004</v>
+      </c>
+      <c r="D11">
+        <v>500</v>
+      </c>
+      <c r="E11">
+        <v>21.29</v>
+      </c>
+      <c r="F11">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>61.08972</v>
+      </c>
+      <c r="C12">
+        <v>149.66889</v>
+      </c>
+      <c r="D12">
+        <v>500</v>
+      </c>
+      <c r="E12">
+        <v>9.32</v>
+      </c>
+      <c r="F12">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>61.08972</v>
+      </c>
+      <c r="C13">
+        <v>149.66889</v>
+      </c>
+      <c r="D13">
+        <v>1067</v>
+      </c>
+      <c r="E13">
+        <v>5.13</v>
+      </c>
+      <c r="F13">
+        <v>9.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C14">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D14">
+        <v>3500</v>
+      </c>
+      <c r="E14">
+        <v>-11.12</v>
+      </c>
+      <c r="F14">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C15">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D15">
+        <v>1500</v>
+      </c>
+      <c r="E15">
+        <v>5.63</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C16">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D16">
+        <v>4500</v>
+      </c>
+      <c r="E16">
+        <v>-20.78</v>
+      </c>
+      <c r="F16">
+        <v>13.58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C17">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D17">
+        <v>2500</v>
+      </c>
+      <c r="E17">
+        <v>-2.12</v>
+      </c>
+      <c r="F17">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C18">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D18">
+        <v>5500</v>
+      </c>
+      <c r="E18">
+        <v>-30.8</v>
+      </c>
+      <c r="F18">
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C19">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D19">
+        <v>6194</v>
+      </c>
+      <c r="E19">
+        <v>-37.65</v>
+      </c>
+      <c r="F19">
+        <v>23.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C20">
+        <v>151.00693999999999</v>
+      </c>
+      <c r="D20">
+        <v>500</v>
+      </c>
+      <c r="E20">
+        <v>12.43</v>
+      </c>
+      <c r="F20">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>36.578330000000001</v>
+      </c>
+      <c r="C21">
+        <v>118.29222</v>
+      </c>
+      <c r="D21">
+        <v>4418</v>
+      </c>
+      <c r="E21">
+        <v>-1.28</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>36.578330000000001</v>
+      </c>
+      <c r="C22">
+        <v>118.29222</v>
+      </c>
+      <c r="D22">
+        <v>3500</v>
+      </c>
+      <c r="E22">
+        <v>7.77</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>36.578330000000001</v>
+      </c>
+      <c r="C23">
+        <v>118.29222</v>
+      </c>
+      <c r="D23">
+        <v>1500</v>
+      </c>
+      <c r="E23">
+        <v>22.93</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>36.578330000000001</v>
+      </c>
+      <c r="C24">
+        <v>118.29222</v>
+      </c>
+      <c r="D24">
+        <v>2500</v>
+      </c>
+      <c r="E24">
+        <v>15.78</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>27.988060000000001</v>
+      </c>
+      <c r="C25">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="D25">
+        <v>6000</v>
+      </c>
+      <c r="E25">
+        <v>-4.26</v>
+      </c>
+      <c r="F25">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>27.988060000000001</v>
+      </c>
+      <c r="C26">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="D26">
+        <v>8850</v>
+      </c>
+      <c r="E26">
+        <v>-28.09</v>
+      </c>
+      <c r="F26">
+        <v>20.29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>27.988060000000001</v>
+      </c>
+      <c r="C27">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>3.29</v>
+      </c>
+      <c r="F27">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>27.988060000000001</v>
+      </c>
+      <c r="C28">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="D28">
+        <v>8000</v>
+      </c>
+      <c r="E28">
+        <v>-20.65</v>
+      </c>
+      <c r="F28">
+        <v>17.649999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>27.988060000000001</v>
+      </c>
+      <c r="C29">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="D29">
+        <v>7000</v>
+      </c>
+      <c r="E29">
+        <v>-12.18</v>
+      </c>
+      <c r="F29">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>27.988060000000001</v>
+      </c>
+      <c r="C30">
+        <v>86.924999999999997</v>
+      </c>
+      <c r="D30">
+        <v>4000</v>
+      </c>
+      <c r="E30">
+        <v>10.32</v>
+      </c>
+      <c r="F30">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C31">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D31">
+        <v>5500</v>
+      </c>
+      <c r="E31">
+        <v>-8.56</v>
+      </c>
+      <c r="F31">
+        <v>11.76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C32">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D32">
+        <v>6500</v>
+      </c>
+      <c r="E32">
+        <v>-18.03</v>
+      </c>
+      <c r="F32">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C33">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D33">
+        <v>8125</v>
+      </c>
+      <c r="E33">
+        <v>-34.5</v>
+      </c>
+      <c r="F33">
+        <v>21.62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C34">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D34">
+        <v>2500</v>
+      </c>
+      <c r="E34">
+        <v>16.53</v>
+      </c>
+      <c r="F34">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C35">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D35">
+        <v>3500</v>
+      </c>
+      <c r="E35">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="F35">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C36">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D36">
+        <v>4500</v>
+      </c>
+      <c r="E36">
+        <v>0.79</v>
+      </c>
+      <c r="F36">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>35.237200000000001</v>
+      </c>
+      <c r="C37">
+        <v>74.588899999999995</v>
+      </c>
+      <c r="D37">
+        <v>7500</v>
+      </c>
+      <c r="E37">
+        <v>-28.24</v>
+      </c>
+      <c r="F37">
+        <v>19.260000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C38">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D38">
+        <v>8000</v>
+      </c>
+      <c r="E38">
+        <v>-20.47</v>
+      </c>
+      <c r="F38">
+        <v>23.97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C39">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D39">
+        <v>3000</v>
+      </c>
+      <c r="E39">
+        <v>15.47</v>
+      </c>
+      <c r="F39">
+        <v>8.09</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C40">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D40">
+        <v>4000</v>
+      </c>
+      <c r="E40">
+        <v>9.18</v>
+      </c>
+      <c r="F40">
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C41">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D41">
+        <v>6000</v>
+      </c>
+      <c r="E41">
+        <v>-5.0599999999999996</v>
+      </c>
+      <c r="F41">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C42">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D42">
+        <v>5000</v>
+      </c>
+      <c r="E42">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="F42">
+        <v>11.91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C43">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D43">
+        <v>7000</v>
+      </c>
+      <c r="E43">
+        <v>-12.62</v>
+      </c>
+      <c r="F43">
+        <v>19.559999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C44">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D44">
+        <v>2000</v>
+      </c>
+      <c r="E44">
+        <v>22.24</v>
+      </c>
+      <c r="F44">
+        <v>8.09</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45">
+        <v>27.702220000000001</v>
+      </c>
+      <c r="C45">
+        <v>88.147499999999994</v>
+      </c>
+      <c r="D45">
+        <v>8586</v>
+      </c>
+      <c r="E45">
+        <v>-25.12</v>
+      </c>
+      <c r="F45">
+        <v>26.62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>27.962499999999999</v>
+      </c>
+      <c r="C46">
+        <v>86.933329999999998</v>
+      </c>
+      <c r="D46">
+        <v>8516</v>
+      </c>
+      <c r="E46">
+        <v>-25.03</v>
+      </c>
+      <c r="F46">
+        <v>18.97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47">
+        <v>27.962499999999999</v>
+      </c>
+      <c r="C47">
+        <v>86.933329999999998</v>
+      </c>
+      <c r="D47">
+        <v>8000</v>
+      </c>
+      <c r="E47">
+        <v>-20.62</v>
+      </c>
+      <c r="F47">
+        <v>17.350000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48">
+        <v>27.962499999999999</v>
+      </c>
+      <c r="C48">
+        <v>86.933329999999998</v>
+      </c>
+      <c r="D48">
+        <v>6000</v>
+      </c>
+      <c r="E48">
+        <v>-4.24</v>
+      </c>
+      <c r="F48">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49">
+        <v>27.962499999999999</v>
+      </c>
+      <c r="C49">
+        <v>86.933329999999998</v>
+      </c>
+      <c r="D49">
+        <v>4000</v>
+      </c>
+      <c r="E49">
+        <v>10.32</v>
+      </c>
+      <c r="F49">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50">
+        <v>27.962499999999999</v>
+      </c>
+      <c r="C50">
+        <v>86.933329999999998</v>
+      </c>
+      <c r="D50">
+        <v>5000</v>
+      </c>
+      <c r="E50">
+        <v>3.21</v>
+      </c>
+      <c r="F50">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51">
+        <v>27.962499999999999</v>
+      </c>
+      <c r="C51">
+        <v>86.933329999999998</v>
+      </c>
+      <c r="D51">
+        <v>7000</v>
+      </c>
+      <c r="E51">
+        <v>-12.18</v>
+      </c>
+      <c r="F51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C52">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D52">
+        <v>4500</v>
+      </c>
+      <c r="E52">
+        <v>4.68</v>
+      </c>
+      <c r="F52">
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C53">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D53">
+        <v>2500</v>
+      </c>
+      <c r="E53">
+        <v>18.62</v>
+      </c>
+      <c r="F53">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C54">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D54">
+        <v>1500</v>
+      </c>
+      <c r="E54">
+        <v>25.21</v>
+      </c>
+      <c r="F54">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C55">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D55">
+        <v>7500</v>
+      </c>
+      <c r="E55">
+        <v>-18.59</v>
+      </c>
+      <c r="F55">
+        <v>19.559999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C56">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D56">
+        <v>6500</v>
+      </c>
+      <c r="E56">
+        <v>-10.38</v>
+      </c>
+      <c r="F56">
+        <v>16.760000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C57">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D57">
+        <v>5500</v>
+      </c>
+      <c r="E57">
+        <v>-2.76</v>
+      </c>
+      <c r="F57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C58">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D58">
+        <v>8167</v>
+      </c>
+      <c r="E58">
+        <v>-24</v>
+      </c>
+      <c r="F58">
+        <v>22.35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59">
+        <v>28.698060000000002</v>
+      </c>
+      <c r="C59">
+        <v>83.487499999999997</v>
+      </c>
+      <c r="D59">
+        <v>3500</v>
+      </c>
+      <c r="E59">
+        <v>11.74</v>
+      </c>
+      <c r="F59">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60">
+        <v>27.86167</v>
+      </c>
+      <c r="C60">
+        <v>86.860280000000003</v>
+      </c>
+      <c r="D60">
+        <v>5000</v>
+      </c>
+      <c r="E60">
+        <v>2.56</v>
+      </c>
+      <c r="F60">
+        <v>11.47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61">
+        <v>27.86167</v>
+      </c>
+      <c r="C61">
+        <v>86.860280000000003</v>
+      </c>
+      <c r="D61">
+        <v>6856</v>
+      </c>
+      <c r="E61">
+        <v>-10.88</v>
+      </c>
+      <c r="F61">
+        <v>14.12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62">
+        <v>27.86167</v>
+      </c>
+      <c r="C62">
+        <v>86.860280000000003</v>
+      </c>
+      <c r="D62">
+        <v>4000</v>
+      </c>
+      <c r="E62">
+        <v>9.56</v>
+      </c>
+      <c r="F62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63">
+        <v>27.86167</v>
+      </c>
+      <c r="C63">
+        <v>86.860280000000003</v>
+      </c>
+      <c r="D63">
+        <v>6000</v>
+      </c>
+      <c r="E63">
+        <v>-4.53</v>
+      </c>
+      <c r="F63">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64">
+        <v>27.86167</v>
+      </c>
+      <c r="C64">
+        <v>86.860280000000003</v>
+      </c>
+      <c r="D64">
+        <v>3000</v>
+      </c>
+      <c r="E64">
+        <v>16.29</v>
+      </c>
+      <c r="F64">
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65">
+        <v>27.891940000000002</v>
+      </c>
+      <c r="C65">
+        <v>87.088610000000003</v>
+      </c>
+      <c r="D65">
+        <v>8462</v>
+      </c>
+      <c r="E65">
+        <v>-23.79</v>
+      </c>
+      <c r="F65">
+        <v>19.71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66">
+        <v>27.891940000000002</v>
+      </c>
+      <c r="C66">
+        <v>87.088610000000003</v>
+      </c>
+      <c r="D66">
+        <v>7500</v>
+      </c>
+      <c r="E66">
+        <v>-15.74</v>
+      </c>
+      <c r="F66">
+        <v>15.88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67">
+        <v>27.891940000000002</v>
+      </c>
+      <c r="C67">
+        <v>87.088610000000003</v>
+      </c>
+      <c r="D67">
+        <v>2500</v>
+      </c>
+      <c r="E67">
+        <v>19.18</v>
+      </c>
+      <c r="F67">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>49</v>
+      </c>
+      <c r="B68">
+        <v>27.891940000000002</v>
+      </c>
+      <c r="C68">
+        <v>87.088610000000003</v>
+      </c>
+      <c r="D68">
+        <v>6500</v>
+      </c>
+      <c r="E68">
+        <v>-8.1199999999999992</v>
+      </c>
+      <c r="F68">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>49</v>
+      </c>
+      <c r="B69">
+        <v>27.891940000000002</v>
+      </c>
+      <c r="C69">
+        <v>87.088610000000003</v>
+      </c>
+      <c r="D69">
+        <v>3500</v>
+      </c>
+      <c r="E69">
+        <v>12.79</v>
+      </c>
+      <c r="F69">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70">
+        <v>27.891940000000002</v>
+      </c>
+      <c r="C70">
+        <v>87.088610000000003</v>
+      </c>
+      <c r="D70">
+        <v>4500</v>
+      </c>
+      <c r="E70">
+        <v>6.18</v>
+      </c>
+      <c r="F70">
+        <v>8.5299999999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B71">
+        <v>27.920829999999999</v>
+      </c>
+      <c r="C71">
+        <v>86.935559999999995</v>
+      </c>
+      <c r="D71">
+        <v>5500</v>
+      </c>
+      <c r="E71">
+        <v>-0.68</v>
+      </c>
+      <c r="F71">
+        <v>11.62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B72">
+        <v>27.920829999999999</v>
+      </c>
+      <c r="C72">
+        <v>86.935559999999995</v>
+      </c>
+      <c r="D72">
+        <v>4500</v>
+      </c>
+      <c r="E72">
+        <v>6.65</v>
+      </c>
+      <c r="F72">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>51</v>
+      </c>
+      <c r="B73">
+        <v>27.920829999999999</v>
+      </c>
+      <c r="C73">
+        <v>86.935559999999995</v>
+      </c>
+      <c r="D73">
+        <v>6183</v>
+      </c>
+      <c r="E73">
+        <v>-5.71</v>
+      </c>
+      <c r="F73">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74">
+        <v>27.920829999999999</v>
+      </c>
+      <c r="C74">
+        <v>86.935559999999995</v>
+      </c>
+      <c r="D74">
+        <v>3500</v>
+      </c>
+      <c r="E74">
+        <v>13.47</v>
+      </c>
+      <c r="F74">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75">
+        <v>28.095829999999999</v>
+      </c>
+      <c r="C75">
+        <v>86.659170000000003</v>
+      </c>
+      <c r="D75">
+        <v>4500</v>
+      </c>
+      <c r="E75">
+        <v>6.74</v>
+      </c>
+      <c r="F75">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76">
+        <v>28.095829999999999</v>
+      </c>
+      <c r="C76">
+        <v>86.659170000000003</v>
+      </c>
+      <c r="D76">
+        <v>8201</v>
+      </c>
+      <c r="E76">
+        <v>-23.71</v>
+      </c>
+      <c r="F76">
+        <v>22.21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77">
+        <v>28.095829999999999</v>
+      </c>
+      <c r="C77">
+        <v>86.659170000000003</v>
+      </c>
+      <c r="D77">
+        <v>5500</v>
+      </c>
+      <c r="E77">
+        <v>-1.03</v>
+      </c>
+      <c r="F77">
+        <v>14.71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>53</v>
+      </c>
+      <c r="B78">
+        <v>28.095829999999999</v>
+      </c>
+      <c r="C78">
+        <v>86.659170000000003</v>
+      </c>
+      <c r="D78">
+        <v>7500</v>
+      </c>
+      <c r="E78">
+        <v>-17.559999999999999</v>
+      </c>
+      <c r="F78">
+        <v>20.149999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79">
+        <v>28.095829999999999</v>
+      </c>
+      <c r="C79">
+        <v>86.659170000000003</v>
+      </c>
+      <c r="D79">
+        <v>6500</v>
+      </c>
+      <c r="E79">
+        <v>-9</v>
+      </c>
+      <c r="F79">
+        <v>17.21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>55</v>
+      </c>
+      <c r="B80">
+        <v>28.353059999999999</v>
+      </c>
+      <c r="C80">
+        <v>85.778890000000004</v>
+      </c>
+      <c r="D80">
+        <v>7500</v>
+      </c>
+      <c r="E80">
+        <v>-17.149999999999999</v>
+      </c>
+      <c r="F80">
+        <v>19.559999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81">
+        <v>28.353059999999999</v>
+      </c>
+      <c r="C81">
+        <v>85.778890000000004</v>
+      </c>
+      <c r="D81">
+        <v>4500</v>
+      </c>
+      <c r="E81">
+        <v>6.94</v>
+      </c>
+      <c r="F81">
+        <v>11.47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>28.353059999999999</v>
+      </c>
+      <c r="C82">
+        <v>85.778890000000004</v>
+      </c>
+      <c r="D82">
+        <v>5500</v>
+      </c>
+      <c r="E82">
+        <v>-0.68</v>
+      </c>
+      <c r="F82">
+        <v>13.24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>55</v>
+      </c>
+      <c r="B83">
+        <v>28.353059999999999</v>
+      </c>
+      <c r="C83">
+        <v>85.778890000000004</v>
+      </c>
+      <c r="D83">
+        <v>6500</v>
+      </c>
+      <c r="E83">
+        <v>-8.56</v>
+      </c>
+      <c r="F83">
+        <v>16.47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>55</v>
+      </c>
+      <c r="B84">
+        <v>28.353059999999999</v>
+      </c>
+      <c r="C84">
+        <v>85.778890000000004</v>
+      </c>
+      <c r="D84">
+        <v>8013</v>
+      </c>
+      <c r="E84">
+        <v>-21.79</v>
+      </c>
+      <c r="F84">
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C85">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D85">
+        <v>3500</v>
+      </c>
+      <c r="E85">
+        <v>11.79</v>
+      </c>
+      <c r="F85">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C86">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D86">
+        <v>7500</v>
+      </c>
+      <c r="E86">
+        <v>-15.71</v>
+      </c>
+      <c r="F86">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C87">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D87">
+        <v>5500</v>
+      </c>
+      <c r="E87">
+        <v>-1.56</v>
+      </c>
+      <c r="F87">
+        <v>11.03</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C88">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D88">
+        <v>2500</v>
+      </c>
+      <c r="E88">
+        <v>18.18</v>
+      </c>
+      <c r="F88">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>57</v>
+      </c>
+      <c r="B89">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C89">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D89">
+        <v>8156</v>
+      </c>
+      <c r="E89">
+        <v>-20.71</v>
+      </c>
+      <c r="F89">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>57</v>
+      </c>
+      <c r="B90">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C90">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D90">
+        <v>4500</v>
+      </c>
+      <c r="E90">
+        <v>5.29</v>
+      </c>
+      <c r="F90">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C91">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D91">
+        <v>6500</v>
+      </c>
+      <c r="E91">
+        <v>-8.4700000000000006</v>
+      </c>
+      <c r="F91">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92">
+        <v>28.551939999999998</v>
+      </c>
+      <c r="C92">
+        <v>84.556669999999997</v>
+      </c>
+      <c r="D92">
+        <v>1500</v>
+      </c>
+      <c r="E92">
+        <v>24.76</v>
+      </c>
+      <c r="F92">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C93">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D93">
+        <v>8091</v>
+      </c>
+      <c r="E93">
+        <v>-21.91</v>
+      </c>
+      <c r="F93">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>59</v>
+      </c>
+      <c r="B94">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C94">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D94">
+        <v>3500</v>
+      </c>
+      <c r="E94">
+        <v>11.71</v>
+      </c>
+      <c r="F94">
+        <v>11.76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>59</v>
+      </c>
+      <c r="B95">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C95">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D95">
+        <v>2500</v>
+      </c>
+      <c r="E95">
+        <v>18.260000000000002</v>
+      </c>
+      <c r="F95">
+        <v>11.76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C96">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D96">
+        <v>7500</v>
+      </c>
+      <c r="E96">
+        <v>-17.239999999999998</v>
+      </c>
+      <c r="F96">
+        <v>16.32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>59</v>
+      </c>
+      <c r="B97">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C97">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D97">
+        <v>6500</v>
+      </c>
+      <c r="E97">
+        <v>-9.65</v>
+      </c>
+      <c r="F97">
+        <v>15.29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+      <c r="B98">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C98">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D98">
+        <v>5500</v>
+      </c>
+      <c r="E98">
+        <v>-2.09</v>
+      </c>
+      <c r="F98">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B99">
+        <v>28.613610000000001</v>
+      </c>
+      <c r="C99">
+        <v>83.871390000000005</v>
+      </c>
+      <c r="D99">
+        <v>4500</v>
+      </c>
+      <c r="E99">
+        <v>4.88</v>
+      </c>
+      <c r="F99">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B100">
+        <v>35.724170000000001</v>
+      </c>
+      <c r="C100">
+        <v>76.696110000000004</v>
+      </c>
+      <c r="D100">
+        <v>5500</v>
+      </c>
+      <c r="E100">
+        <v>-9.9700000000000006</v>
+      </c>
+      <c r="F100">
+        <v>9.7100000000000009</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101">
+        <v>35.724170000000001</v>
+      </c>
+      <c r="C101">
+        <v>76.696110000000004</v>
+      </c>
+      <c r="D101">
+        <v>8068</v>
+      </c>
+      <c r="E101">
+        <v>-32.65</v>
+      </c>
+      <c r="F101">
+        <v>14.26</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>61</v>
+      </c>
+      <c r="B102">
+        <v>35.724170000000001</v>
+      </c>
+      <c r="C102">
+        <v>76.696110000000004</v>
+      </c>
+      <c r="D102">
+        <v>4500</v>
+      </c>
+      <c r="E102">
+        <v>-1.41</v>
+      </c>
+      <c r="F102">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>61</v>
+      </c>
+      <c r="B103">
+        <v>35.724170000000001</v>
+      </c>
+      <c r="C103">
+        <v>76.696110000000004</v>
+      </c>
+      <c r="D103">
+        <v>6500</v>
+      </c>
+      <c r="E103">
+        <v>-18.62</v>
+      </c>
+      <c r="F103">
+        <v>11.03</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104">
+        <v>35.724170000000001</v>
+      </c>
+      <c r="C104">
+        <v>76.696110000000004</v>
+      </c>
+      <c r="D104">
+        <v>7500</v>
+      </c>
+      <c r="E104">
+        <v>-27.44</v>
+      </c>
+      <c r="F104">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>64</v>
+      </c>
+      <c r="B105">
+        <v>35.759169999999997</v>
+      </c>
+      <c r="C105">
+        <v>76.641940000000005</v>
+      </c>
+      <c r="D105">
+        <v>8035</v>
+      </c>
+      <c r="E105">
+        <v>-32.29</v>
+      </c>
+      <c r="F105">
+        <v>14.26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>64</v>
+      </c>
+      <c r="B106">
+        <v>35.759169999999997</v>
+      </c>
+      <c r="C106">
+        <v>76.641940000000005</v>
+      </c>
+      <c r="D106">
+        <v>4500</v>
+      </c>
+      <c r="E106">
+        <v>-1.56</v>
+      </c>
+      <c r="F106">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>64</v>
+      </c>
+      <c r="B107">
+        <v>35.759169999999997</v>
+      </c>
+      <c r="C107">
+        <v>76.641940000000005</v>
+      </c>
+      <c r="D107">
+        <v>7500</v>
+      </c>
+      <c r="E107">
+        <v>-27.59</v>
+      </c>
+      <c r="F107">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>64</v>
+      </c>
+      <c r="B108">
+        <v>35.759169999999997</v>
+      </c>
+      <c r="C108">
+        <v>76.641940000000005</v>
+      </c>
+      <c r="D108">
+        <v>5500</v>
+      </c>
+      <c r="E108">
+        <v>-10.09</v>
+      </c>
+      <c r="F108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>64</v>
+      </c>
+      <c r="B109">
+        <v>35.759169999999997</v>
+      </c>
+      <c r="C109">
+        <v>76.641940000000005</v>
+      </c>
+      <c r="D109">
+        <v>6500</v>
+      </c>
+      <c r="E109">
+        <v>-18.68</v>
+      </c>
+      <c r="F109">
+        <v>11.03</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>66</v>
+      </c>
+      <c r="B110">
+        <v>35.81306</v>
+      </c>
+      <c r="C110">
+        <v>76.565280000000001</v>
+      </c>
+      <c r="D110">
+        <v>4500</v>
+      </c>
+      <c r="E110">
+        <v>-2.09</v>
+      </c>
+      <c r="F110">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>66</v>
+      </c>
+      <c r="B111">
+        <v>35.81306</v>
+      </c>
+      <c r="C111">
+        <v>76.565280000000001</v>
+      </c>
+      <c r="D111">
+        <v>7500</v>
+      </c>
+      <c r="E111">
+        <v>-28.29</v>
+      </c>
+      <c r="F111">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>66</v>
+      </c>
+      <c r="B112">
+        <v>35.81306</v>
+      </c>
+      <c r="C112">
+        <v>76.565280000000001</v>
+      </c>
+      <c r="D112">
+        <v>5500</v>
+      </c>
+      <c r="E112">
+        <v>-10.68</v>
+      </c>
+      <c r="F112">
+        <v>10.88</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>66</v>
+      </c>
+      <c r="B113">
+        <v>35.81306</v>
+      </c>
+      <c r="C113">
+        <v>76.565280000000001</v>
+      </c>
+      <c r="D113">
+        <v>8047</v>
+      </c>
+      <c r="E113">
+        <v>-33.35</v>
+      </c>
+      <c r="F113">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>66</v>
+      </c>
+      <c r="B114">
+        <v>35.81306</v>
+      </c>
+      <c r="C114">
+        <v>76.565280000000001</v>
+      </c>
+      <c r="D114">
+        <v>6500</v>
+      </c>
+      <c r="E114">
+        <v>-19.260000000000002</v>
+      </c>
+      <c r="F114">
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>68</v>
+      </c>
+      <c r="B115">
+        <v>35.881390000000003</v>
+      </c>
+      <c r="C115">
+        <v>76.513329999999996</v>
+      </c>
+      <c r="D115">
+        <v>8000</v>
+      </c>
+      <c r="E115">
+        <v>-33.619999999999997</v>
+      </c>
+      <c r="F115">
+        <v>18.239999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>68</v>
+      </c>
+      <c r="B116">
+        <v>35.881390000000003</v>
+      </c>
+      <c r="C116">
+        <v>76.513329999999996</v>
+      </c>
+      <c r="D116">
+        <v>4000</v>
+      </c>
+      <c r="E116">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="F116">
+        <v>9.41</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>68</v>
+      </c>
+      <c r="B117">
+        <v>35.881390000000003</v>
+      </c>
+      <c r="C117">
+        <v>76.513329999999996</v>
+      </c>
+      <c r="D117">
+        <v>7000</v>
+      </c>
+      <c r="E117">
+        <v>-24.41</v>
+      </c>
+      <c r="F117">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>68</v>
+      </c>
+      <c r="B118">
+        <v>35.881390000000003</v>
+      </c>
+      <c r="C118">
+        <v>76.513329999999996</v>
+      </c>
+      <c r="D118">
+        <v>8612</v>
+      </c>
+      <c r="E118">
+        <v>-39.44</v>
+      </c>
+      <c r="F118">
+        <v>20.29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>68</v>
+      </c>
+      <c r="B119">
+        <v>35.881390000000003</v>
+      </c>
+      <c r="C119">
+        <v>76.513329999999996</v>
+      </c>
+      <c r="D119">
+        <v>5000</v>
+      </c>
+      <c r="E119">
+        <v>-6.38</v>
+      </c>
+      <c r="F119">
+        <v>11.47</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>68</v>
+      </c>
+      <c r="B120">
+        <v>35.881390000000003</v>
+      </c>
+      <c r="C120">
+        <v>76.513329999999996</v>
+      </c>
+      <c r="D120">
+        <v>6000</v>
+      </c>
+      <c r="E120">
+        <v>-15.29</v>
+      </c>
+      <c r="F120">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>70</v>
+      </c>
+      <c r="B121">
+        <v>78.633889999999994</v>
+      </c>
+      <c r="C121">
+        <v>85.225279999999998</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>-17.02</v>
+      </c>
+      <c r="F121">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>70</v>
+      </c>
+      <c r="B122">
+        <v>78.633889999999994</v>
+      </c>
+      <c r="C122">
+        <v>85.225279999999998</v>
+      </c>
+      <c r="D122">
+        <v>4897</v>
+      </c>
+      <c r="E122">
+        <v>-59.97</v>
+      </c>
+      <c r="F122">
+        <v>54.67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>70</v>
+      </c>
+      <c r="B123">
+        <v>78.633889999999994</v>
+      </c>
+      <c r="C123">
+        <v>85.225279999999998</v>
+      </c>
+      <c r="D123">
+        <v>2000</v>
+      </c>
+      <c r="E123">
+        <v>-30.45</v>
+      </c>
+      <c r="F123">
+        <v>14.17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>70</v>
+      </c>
+      <c r="B124">
+        <v>78.633889999999994</v>
+      </c>
+      <c r="C124">
+        <v>85.225279999999998</v>
+      </c>
+      <c r="D124">
+        <v>4000</v>
+      </c>
+      <c r="E124">
+        <v>-50.02</v>
+      </c>
+      <c r="F124">
+        <v>38.83</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>70</v>
+      </c>
+      <c r="B125">
+        <v>78.633889999999994</v>
+      </c>
+      <c r="C125">
+        <v>85.225279999999998</v>
+      </c>
+      <c r="D125">
+        <v>1000</v>
+      </c>
+      <c r="E125">
+        <v>-24.88</v>
+      </c>
+      <c r="F125">
+        <v>11.58</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>70</v>
+      </c>
+      <c r="B126">
+        <v>78.633889999999994</v>
+      </c>
+      <c r="C126">
+        <v>85.225279999999998</v>
+      </c>
+      <c r="D126">
+        <v>3000</v>
+      </c>
+      <c r="E126">
+        <v>-38.479999999999997</v>
+      </c>
+      <c r="F126">
+        <v>21.92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add pre-commit hook to prevent large files from being committed
</commit_message>
<xml_diff>
--- a/scrape_mountain_weather_data/analysis/avg_morning_chill_june_2024_excel.xlsx
+++ b/scrape_mountain_weather_data/analysis/avg_morning_chill_june_2024_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmwad\OneDrive\Desktop\repos\scrape-mountain-weather-data\scrape_mountain_weather_data\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0097DAAE-329A-49D4-9035-4CD59BD77114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BB6BEE-06C0-4F55-A2B4-E69F78B06941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{A48DE54E-D8C0-4CF6-92BB-8002D761C2DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{A48DE54E-D8C0-4CF6-92BB-8002D761C2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -268,6 +268,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -745,8 +748,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -11233,7 +11237,7 @@
   <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11270,10 +11274,10 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>45.832500000000003</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>6.8650000000000002</v>
       </c>
       <c r="D2">
@@ -11290,10 +11294,10 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>45.832500000000003</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>6.8650000000000002</v>
       </c>
       <c r="D3">
@@ -11310,10 +11314,10 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>45.832500000000003</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>6.8650000000000002</v>
       </c>
       <c r="D4">
@@ -11330,10 +11334,10 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>45.832500000000003</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>6.8650000000000002</v>
       </c>
       <c r="D5">
@@ -11350,10 +11354,10 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>45.832500000000003</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>6.8650000000000002</v>
       </c>
       <c r="D6">
@@ -11370,10 +11374,10 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>44.27</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>71.303060000000002</v>
       </c>
       <c r="D7">
@@ -11390,10 +11394,10 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>44.27</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>71.303060000000002</v>
       </c>
       <c r="D8">
@@ -11410,10 +11414,10 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>35.765000000000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>82.265280000000004</v>
       </c>
       <c r="D9">
@@ -11430,10 +11434,10 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>35.765000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>82.265280000000004</v>
       </c>
       <c r="D10">
@@ -11450,10 +11454,10 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>35.765000000000001</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>82.265280000000004</v>
       </c>
       <c r="D11">
@@ -11470,10 +11474,10 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>61.08972</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>149.66889</v>
       </c>
       <c r="D12">
@@ -11490,10 +11494,10 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>61.08972</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>149.66889</v>
       </c>
       <c r="D13">
@@ -11510,10 +11514,10 @@
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D14">
@@ -11530,10 +11534,10 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D15">
@@ -11550,10 +11554,10 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D16">
@@ -11570,10 +11574,10 @@
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D17">
@@ -11590,10 +11594,10 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D18">
@@ -11610,10 +11614,10 @@
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D19">
@@ -11630,10 +11634,10 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>63.068890000000003</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>151.00693999999999</v>
       </c>
       <c r="D20">
@@ -11650,10 +11654,10 @@
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>36.578330000000001</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>118.29222</v>
       </c>
       <c r="D21">
@@ -11670,10 +11674,10 @@
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>36.578330000000001</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>118.29222</v>
       </c>
       <c r="D22">
@@ -11690,10 +11694,10 @@
       <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>36.578330000000001</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>118.29222</v>
       </c>
       <c r="D23">
@@ -11710,10 +11714,10 @@
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>36.578330000000001</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>118.29222</v>
       </c>
       <c r="D24">
@@ -11730,10 +11734,10 @@
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>27.988060000000001</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>86.924999999999997</v>
       </c>
       <c r="D25">
@@ -11750,10 +11754,10 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>27.988060000000001</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>86.924999999999997</v>
       </c>
       <c r="D26">
@@ -11770,10 +11774,10 @@
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>27.988060000000001</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>86.924999999999997</v>
       </c>
       <c r="D27">
@@ -11790,10 +11794,10 @@
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>27.988060000000001</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>86.924999999999997</v>
       </c>
       <c r="D28">
@@ -11810,10 +11814,10 @@
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>27.988060000000001</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>86.924999999999997</v>
       </c>
       <c r="D29">
@@ -11830,10 +11834,10 @@
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>27.988060000000001</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>86.924999999999997</v>
       </c>
       <c r="D30">
@@ -11850,10 +11854,10 @@
       <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D31">
@@ -11870,10 +11874,10 @@
       <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D32">
@@ -11890,10 +11894,10 @@
       <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D33">
@@ -11910,10 +11914,10 @@
       <c r="A34" t="s">
         <v>36</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D34">
@@ -11930,10 +11934,10 @@
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D35">
@@ -11950,10 +11954,10 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D36">
@@ -11970,10 +11974,10 @@
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>35.237200000000001</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>74.588899999999995</v>
       </c>
       <c r="D37">
@@ -11990,10 +11994,10 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D38">
@@ -12010,10 +12014,10 @@
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D39">
@@ -12030,10 +12034,10 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D40">
@@ -12050,10 +12054,10 @@
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D41">
@@ -12070,10 +12074,10 @@
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D42">
@@ -12090,10 +12094,10 @@
       <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D43">
@@ -12110,10 +12114,10 @@
       <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D44">
@@ -12130,10 +12134,10 @@
       <c r="A45" t="s">
         <v>39</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>27.702220000000001</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>88.147499999999994</v>
       </c>
       <c r="D45">
@@ -12150,10 +12154,10 @@
       <c r="A46" t="s">
         <v>42</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>27.962499999999999</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>86.933329999999998</v>
       </c>
       <c r="D46">
@@ -12170,10 +12174,10 @@
       <c r="A47" t="s">
         <v>42</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>27.962499999999999</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>86.933329999999998</v>
       </c>
       <c r="D47">
@@ -12190,10 +12194,10 @@
       <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>27.962499999999999</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>86.933329999999998</v>
       </c>
       <c r="D48">
@@ -12210,10 +12214,10 @@
       <c r="A49" t="s">
         <v>42</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>27.962499999999999</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>86.933329999999998</v>
       </c>
       <c r="D49">
@@ -12230,10 +12234,10 @@
       <c r="A50" t="s">
         <v>42</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>27.962499999999999</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>86.933329999999998</v>
       </c>
       <c r="D50">
@@ -12250,10 +12254,10 @@
       <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>27.962499999999999</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>86.933329999999998</v>
       </c>
       <c r="D51">
@@ -12270,10 +12274,10 @@
       <c r="A52" t="s">
         <v>44</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D52">
@@ -12290,10 +12294,10 @@
       <c r="A53" t="s">
         <v>44</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D53">
@@ -12310,10 +12314,10 @@
       <c r="A54" t="s">
         <v>44</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D54">
@@ -12330,10 +12334,10 @@
       <c r="A55" t="s">
         <v>44</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D55">
@@ -12350,10 +12354,10 @@
       <c r="A56" t="s">
         <v>44</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D56">
@@ -12370,10 +12374,10 @@
       <c r="A57" t="s">
         <v>44</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D57">
@@ -12390,10 +12394,10 @@
       <c r="A58" t="s">
         <v>44</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D58">
@@ -12410,10 +12414,10 @@
       <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>28.698060000000002</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <v>83.487499999999997</v>
       </c>
       <c r="D59">
@@ -12430,10 +12434,10 @@
       <c r="A60" t="s">
         <v>47</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>27.86167</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
         <v>86.860280000000003</v>
       </c>
       <c r="D60">
@@ -12450,10 +12454,10 @@
       <c r="A61" t="s">
         <v>47</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>27.86167</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <v>86.860280000000003</v>
       </c>
       <c r="D61">
@@ -12470,10 +12474,10 @@
       <c r="A62" t="s">
         <v>47</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>27.86167</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="1">
         <v>86.860280000000003</v>
       </c>
       <c r="D62">
@@ -12490,10 +12494,10 @@
       <c r="A63" t="s">
         <v>47</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>27.86167</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="1">
         <v>86.860280000000003</v>
       </c>
       <c r="D63">
@@ -12510,10 +12514,10 @@
       <c r="A64" t="s">
         <v>47</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>27.86167</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
         <v>86.860280000000003</v>
       </c>
       <c r="D64">
@@ -12530,10 +12534,10 @@
       <c r="A65" t="s">
         <v>49</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>27.891940000000002</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="1">
         <v>87.088610000000003</v>
       </c>
       <c r="D65">
@@ -12550,10 +12554,10 @@
       <c r="A66" t="s">
         <v>49</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>27.891940000000002</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
         <v>87.088610000000003</v>
       </c>
       <c r="D66">
@@ -12570,10 +12574,10 @@
       <c r="A67" t="s">
         <v>49</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>27.891940000000002</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="1">
         <v>87.088610000000003</v>
       </c>
       <c r="D67">
@@ -12590,10 +12594,10 @@
       <c r="A68" t="s">
         <v>49</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>27.891940000000002</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="1">
         <v>87.088610000000003</v>
       </c>
       <c r="D68">
@@ -12610,10 +12614,10 @@
       <c r="A69" t="s">
         <v>49</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>27.891940000000002</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
         <v>87.088610000000003</v>
       </c>
       <c r="D69">
@@ -12630,10 +12634,10 @@
       <c r="A70" t="s">
         <v>49</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>27.891940000000002</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="1">
         <v>87.088610000000003</v>
       </c>
       <c r="D70">
@@ -12650,10 +12654,10 @@
       <c r="A71" t="s">
         <v>51</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>27.920829999999999</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="1">
         <v>86.935559999999995</v>
       </c>
       <c r="D71">
@@ -12670,10 +12674,10 @@
       <c r="A72" t="s">
         <v>51</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>27.920829999999999</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="1">
         <v>86.935559999999995</v>
       </c>
       <c r="D72">
@@ -12690,10 +12694,10 @@
       <c r="A73" t="s">
         <v>51</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>27.920829999999999</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="1">
         <v>86.935559999999995</v>
       </c>
       <c r="D73">
@@ -12710,10 +12714,10 @@
       <c r="A74" t="s">
         <v>51</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>27.920829999999999</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="1">
         <v>86.935559999999995</v>
       </c>
       <c r="D74">
@@ -12730,10 +12734,10 @@
       <c r="A75" t="s">
         <v>53</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>28.095829999999999</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="1">
         <v>86.659170000000003</v>
       </c>
       <c r="D75">
@@ -12750,10 +12754,10 @@
       <c r="A76" t="s">
         <v>53</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>28.095829999999999</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="1">
         <v>86.659170000000003</v>
       </c>
       <c r="D76">
@@ -12770,10 +12774,10 @@
       <c r="A77" t="s">
         <v>53</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>28.095829999999999</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="1">
         <v>86.659170000000003</v>
       </c>
       <c r="D77">
@@ -12790,10 +12794,10 @@
       <c r="A78" t="s">
         <v>53</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>28.095829999999999</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="1">
         <v>86.659170000000003</v>
       </c>
       <c r="D78">
@@ -12810,10 +12814,10 @@
       <c r="A79" t="s">
         <v>53</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>28.095829999999999</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="1">
         <v>86.659170000000003</v>
       </c>
       <c r="D79">
@@ -12830,10 +12834,10 @@
       <c r="A80" t="s">
         <v>55</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>28.353059999999999</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="1">
         <v>85.778890000000004</v>
       </c>
       <c r="D80">
@@ -12850,10 +12854,10 @@
       <c r="A81" t="s">
         <v>55</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>28.353059999999999</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="1">
         <v>85.778890000000004</v>
       </c>
       <c r="D81">
@@ -12870,10 +12874,10 @@
       <c r="A82" t="s">
         <v>55</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>28.353059999999999</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="1">
         <v>85.778890000000004</v>
       </c>
       <c r="D82">
@@ -12890,10 +12894,10 @@
       <c r="A83" t="s">
         <v>55</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>28.353059999999999</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="1">
         <v>85.778890000000004</v>
       </c>
       <c r="D83">
@@ -12910,10 +12914,10 @@
       <c r="A84" t="s">
         <v>55</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>28.353059999999999</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="1">
         <v>85.778890000000004</v>
       </c>
       <c r="D84">
@@ -12930,10 +12934,10 @@
       <c r="A85" t="s">
         <v>57</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D85">
@@ -12950,10 +12954,10 @@
       <c r="A86" t="s">
         <v>57</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D86">
@@ -12970,10 +12974,10 @@
       <c r="A87" t="s">
         <v>57</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D87">
@@ -12990,10 +12994,10 @@
       <c r="A88" t="s">
         <v>57</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D88">
@@ -13010,10 +13014,10 @@
       <c r="A89" t="s">
         <v>57</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D89">
@@ -13030,10 +13034,10 @@
       <c r="A90" t="s">
         <v>57</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D90">
@@ -13050,10 +13054,10 @@
       <c r="A91" t="s">
         <v>57</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D91">
@@ -13070,10 +13074,10 @@
       <c r="A92" t="s">
         <v>57</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>28.551939999999998</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="1">
         <v>84.556669999999997</v>
       </c>
       <c r="D92">
@@ -13090,10 +13094,10 @@
       <c r="A93" t="s">
         <v>59</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D93">
@@ -13110,10 +13114,10 @@
       <c r="A94" t="s">
         <v>59</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D94">
@@ -13130,10 +13134,10 @@
       <c r="A95" t="s">
         <v>59</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D95">
@@ -13150,10 +13154,10 @@
       <c r="A96" t="s">
         <v>59</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D96">
@@ -13170,10 +13174,10 @@
       <c r="A97" t="s">
         <v>59</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D97">
@@ -13190,10 +13194,10 @@
       <c r="A98" t="s">
         <v>59</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D98">
@@ -13210,10 +13214,10 @@
       <c r="A99" t="s">
         <v>59</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>28.613610000000001</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="1">
         <v>83.871390000000005</v>
       </c>
       <c r="D99">
@@ -13230,10 +13234,10 @@
       <c r="A100" t="s">
         <v>61</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>35.724170000000001</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="1">
         <v>76.696110000000004</v>
       </c>
       <c r="D100">
@@ -13250,10 +13254,10 @@
       <c r="A101" t="s">
         <v>61</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>35.724170000000001</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="1">
         <v>76.696110000000004</v>
       </c>
       <c r="D101">
@@ -13270,10 +13274,10 @@
       <c r="A102" t="s">
         <v>61</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>35.724170000000001</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="1">
         <v>76.696110000000004</v>
       </c>
       <c r="D102">
@@ -13290,10 +13294,10 @@
       <c r="A103" t="s">
         <v>61</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
         <v>35.724170000000001</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="1">
         <v>76.696110000000004</v>
       </c>
       <c r="D103">
@@ -13310,10 +13314,10 @@
       <c r="A104" t="s">
         <v>61</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="1">
         <v>35.724170000000001</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="1">
         <v>76.696110000000004</v>
       </c>
       <c r="D104">
@@ -13330,10 +13334,10 @@
       <c r="A105" t="s">
         <v>64</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
         <v>35.759169999999997</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="1">
         <v>76.641940000000005</v>
       </c>
       <c r="D105">
@@ -13350,10 +13354,10 @@
       <c r="A106" t="s">
         <v>64</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>35.759169999999997</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="1">
         <v>76.641940000000005</v>
       </c>
       <c r="D106">
@@ -13370,10 +13374,10 @@
       <c r="A107" t="s">
         <v>64</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>35.759169999999997</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="1">
         <v>76.641940000000005</v>
       </c>
       <c r="D107">
@@ -13390,10 +13394,10 @@
       <c r="A108" t="s">
         <v>64</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="1">
         <v>35.759169999999997</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="1">
         <v>76.641940000000005</v>
       </c>
       <c r="D108">
@@ -13410,10 +13414,10 @@
       <c r="A109" t="s">
         <v>64</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="1">
         <v>35.759169999999997</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="1">
         <v>76.641940000000005</v>
       </c>
       <c r="D109">
@@ -13430,10 +13434,10 @@
       <c r="A110" t="s">
         <v>66</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="1">
         <v>35.81306</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="1">
         <v>76.565280000000001</v>
       </c>
       <c r="D110">
@@ -13450,10 +13454,10 @@
       <c r="A111" t="s">
         <v>66</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="1">
         <v>35.81306</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="1">
         <v>76.565280000000001</v>
       </c>
       <c r="D111">
@@ -13470,10 +13474,10 @@
       <c r="A112" t="s">
         <v>66</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="1">
         <v>35.81306</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="1">
         <v>76.565280000000001</v>
       </c>
       <c r="D112">
@@ -13490,10 +13494,10 @@
       <c r="A113" t="s">
         <v>66</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="1">
         <v>35.81306</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="1">
         <v>76.565280000000001</v>
       </c>
       <c r="D113">
@@ -13510,10 +13514,10 @@
       <c r="A114" t="s">
         <v>66</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>35.81306</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="1">
         <v>76.565280000000001</v>
       </c>
       <c r="D114">
@@ -13530,10 +13534,10 @@
       <c r="A115" t="s">
         <v>68</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="1">
         <v>35.881390000000003</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="1">
         <v>76.513329999999996</v>
       </c>
       <c r="D115">
@@ -13550,10 +13554,10 @@
       <c r="A116" t="s">
         <v>68</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="1">
         <v>35.881390000000003</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="1">
         <v>76.513329999999996</v>
       </c>
       <c r="D116">
@@ -13570,10 +13574,10 @@
       <c r="A117" t="s">
         <v>68</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>35.881390000000003</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="1">
         <v>76.513329999999996</v>
       </c>
       <c r="D117">
@@ -13590,10 +13594,10 @@
       <c r="A118" t="s">
         <v>68</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>35.881390000000003</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="1">
         <v>76.513329999999996</v>
       </c>
       <c r="D118">
@@ -13610,10 +13614,10 @@
       <c r="A119" t="s">
         <v>68</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>35.881390000000003</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="1">
         <v>76.513329999999996</v>
       </c>
       <c r="D119">
@@ -13630,10 +13634,10 @@
       <c r="A120" t="s">
         <v>68</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="1">
         <v>35.881390000000003</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="1">
         <v>76.513329999999996</v>
       </c>
       <c r="D120">
@@ -13650,10 +13654,10 @@
       <c r="A121" t="s">
         <v>70</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>78.633889999999994</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="1">
         <v>85.225279999999998</v>
       </c>
       <c r="D121">
@@ -13670,10 +13674,10 @@
       <c r="A122" t="s">
         <v>70</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>78.633889999999994</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="1">
         <v>85.225279999999998</v>
       </c>
       <c r="D122">
@@ -13690,10 +13694,10 @@
       <c r="A123" t="s">
         <v>70</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>78.633889999999994</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="1">
         <v>85.225279999999998</v>
       </c>
       <c r="D123">
@@ -13710,10 +13714,10 @@
       <c r="A124" t="s">
         <v>70</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="1">
         <v>78.633889999999994</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="1">
         <v>85.225279999999998</v>
       </c>
       <c r="D124">
@@ -13730,10 +13734,10 @@
       <c r="A125" t="s">
         <v>70</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="1">
         <v>78.633889999999994</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="1">
         <v>85.225279999999998</v>
       </c>
       <c r="D125">
@@ -13750,10 +13754,10 @@
       <c r="A126" t="s">
         <v>70</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="1">
         <v>78.633889999999994</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="1">
         <v>85.225279999999998</v>
       </c>
       <c r="D126">
@@ -13768,5 +13772,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add analysis of prediction plots w time_diff truncated to <= 125 hours
</commit_message>
<xml_diff>
--- a/scrape_mountain_weather_data/analysis/avg_morning_chill_june_2024_excel.xlsx
+++ b/scrape_mountain_weather_data/analysis/avg_morning_chill_june_2024_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmwad\OneDrive\Desktop\repos\scrape-mountain-weather-data\scrape_mountain_weather_data\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BB6BEE-06C0-4F55-A2B4-E69F78B06941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651B4384-7911-4318-8D6B-D316E5A0ACBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{A48DE54E-D8C0-4CF6-92BB-8002D761C2DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A48DE54E-D8C0-4CF6-92BB-8002D761C2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="82">
   <si>
     <t>mtn_name</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>61.08972,-149.66889</t>
+  </si>
+  <si>
+    <t>elevation (m)</t>
+  </si>
+  <si>
+    <t>average chill (degrees C)</t>
+  </si>
+  <si>
+    <t>average wind speed (km/h)</t>
   </si>
 </sst>
 </file>
@@ -911,22 +920,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7000</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>8612</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -938,22 +947,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-24.41</c:v>
+                  <c:v>2.23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.29</c:v>
+                  <c:v>-6.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-39.44</c:v>
+                  <c:v>-15.27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.38</c:v>
+                  <c:v>-24.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2599999999999998</c:v>
+                  <c:v>-33.58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-33.619999999999997</c:v>
+                  <c:v>-39.450000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,85 +1268,85 @@
                   <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4500</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>5500</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8068</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4500</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>6500</c:v>
+                  <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7500</c:v>
+                  <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7500</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5500</c:v>
+                  <c:v>6500</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8035</c:v>
+                  <c:v>6500</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4500</c:v>
+                  <c:v>6500</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>6500</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4500</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6500</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8047</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5500</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7000</c:v>
+                  <c:v>8035</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6000</c:v>
+                  <c:v>8068</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>8047</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8125</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>8612</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1349,88 +1358,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>16.53</c:v>
+                  <c:v>16.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79</c:v>
+                  <c:v>9.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.56</c:v>
+                  <c:v>2.23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-18.03</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-28.24</c:v>
+                  <c:v>-1.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3800000000000008</c:v>
+                  <c:v>-1.55</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-34.5</c:v>
+                  <c:v>-2.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-32.65</c:v>
+                  <c:v>-6.37</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.41</c:v>
+                  <c:v>-8.67</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-18.62</c:v>
+                  <c:v>-9.9499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-27.44</c:v>
+                  <c:v>-10.07</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-9.9700000000000006</c:v>
+                  <c:v>-10.65</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-27.59</c:v>
+                  <c:v>-15.27</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-10.09</c:v>
+                  <c:v>-18.079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-32.29</c:v>
+                  <c:v>-18.63</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.56</c:v>
+                  <c:v>-18.68</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-18.68</c:v>
+                  <c:v>-19.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.09</c:v>
+                  <c:v>-24.38</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-19.260000000000002</c:v>
+                  <c:v>-27.45</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-33.35</c:v>
+                  <c:v>-27.58</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-10.68</c:v>
+                  <c:v>-28.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-28.29</c:v>
+                  <c:v>-28.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-24.41</c:v>
+                  <c:v>-32.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-15.29</c:v>
+                  <c:v>-32.67</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-39.44</c:v>
+                  <c:v>-33.32</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-6.38</c:v>
+                  <c:v>-33.58</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2599999999999998</c:v>
+                  <c:v>-34.549999999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-33.619999999999997</c:v>
+                  <c:v>-39.450000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1726,51 +1735,51 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'chill at 4-4500m vs. abs. lat'!$B$2:$B$20</c:f>
+              <c:f>'chill at 4-4500m vs. abs. lat'!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>45.832500000000003</c:v>
+                  <c:v>27.988060000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.068890000000003</c:v>
+                  <c:v>27.962499999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>27.86167</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.702220000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.353059999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.095829999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.920829999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.891940000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.551939999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.613610000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.698060000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35.881390000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35.237200000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>36.578330000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27.988060000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.237200000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27.702220000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27.962499999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28.698060000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27.86167</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>27.920829999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>28.095829999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>28.353059999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>28.551939999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>28.613610000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>35.724170000000001</c:v>
@@ -1782,9 +1791,12 @@
                   <c:v>35.81306</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35.881390000000003</c:v>
+                  <c:v>45.832500000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>63.068890000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>78.633889999999994</c:v>
                 </c:pt>
               </c:numCache>
@@ -1792,65 +1804,68 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'chill at 4-4500m vs. abs. lat'!$C$2:$C$20</c:f>
+              <c:f>'chill at 4-4500m vs. abs. lat'!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-10.32</c:v>
+                  <c:v>10.27</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-10.15</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>-20.78</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1.28</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.79</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.18</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.32</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.56</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.65</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.74</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.94</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.88</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.41</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-1.56</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-2.09</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.2599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>-50.02</c:v>
                 </c:pt>
               </c:numCache>
@@ -2050,6 +2065,433 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.42276127331756308"/>
+                  <c:y val="-0.11149484197782042"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'chill vs. avg. windspeed'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.67</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.67</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.33</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.83</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.58</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>38.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'chill vs. avg. windspeed'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-10.15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-20.78</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-50.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4160-4BCC-A8EB-83DE8F5EBDB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1108767663"/>
+        <c:axId val="1108758543"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1108767663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1108758543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1108758543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1108767663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2131,6 +2573,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3718,6 +4200,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3821,6 +4819,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47E838ED-44B0-E1E2-A08B-4756E9655337}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>173355</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60006</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A285521-FE37-424E-F24F-91DBC05B47FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9138,13 +10177,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
@@ -9157,10 +10197,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -9168,10 +10208,10 @@
         <v>68</v>
       </c>
       <c r="B2">
-        <v>7000</v>
+        <v>4000</v>
       </c>
       <c r="C2">
-        <v>-24.41</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9179,10 +10219,10 @@
         <v>68</v>
       </c>
       <c r="B3">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="C3">
-        <v>-15.29</v>
+        <v>-6.37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -9190,10 +10230,10 @@
         <v>68</v>
       </c>
       <c r="B4">
-        <v>8612</v>
+        <v>6000</v>
       </c>
       <c r="C4">
-        <v>-39.44</v>
+        <v>-15.27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -9201,10 +10241,10 @@
         <v>68</v>
       </c>
       <c r="B5">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="C5">
-        <v>-6.38</v>
+        <v>-24.38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9212,10 +10252,10 @@
         <v>68</v>
       </c>
       <c r="B6">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="C6">
-        <v>2.2599999999999998</v>
+        <v>-33.58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -9223,10 +10263,10 @@
         <v>68</v>
       </c>
       <c r="B7">
-        <v>8000</v>
+        <v>8612</v>
       </c>
       <c r="C7">
-        <v>-33.619999999999997</v>
+        <v>-39.450000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -9240,14 +10280,14 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -9258,10 +10298,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -9272,7 +10312,7 @@
         <v>2500</v>
       </c>
       <c r="C2">
-        <v>16.53</v>
+        <v>16.28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9280,21 +10320,21 @@
         <v>36</v>
       </c>
       <c r="B3">
-        <v>4500</v>
+        <v>3500</v>
       </c>
       <c r="C3">
-        <v>0.79</v>
+        <v>9.08</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B4">
-        <v>5500</v>
+        <v>4000</v>
       </c>
       <c r="C4">
-        <v>-8.56</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -9302,65 +10342,65 @@
         <v>36</v>
       </c>
       <c r="B5">
-        <v>6500</v>
+        <v>4500</v>
       </c>
       <c r="C5">
-        <v>-18.03</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B6">
-        <v>7500</v>
+        <v>4500</v>
       </c>
       <c r="C6">
-        <v>-28.24</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B7">
-        <v>3500</v>
+        <v>4500</v>
       </c>
       <c r="C7">
-        <v>9.3800000000000008</v>
+        <v>-1.55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B8">
-        <v>8125</v>
+        <v>4500</v>
       </c>
       <c r="C8">
-        <v>-34.5</v>
+        <v>-2.08</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B9">
-        <v>8068</v>
+        <v>5000</v>
       </c>
       <c r="C9">
-        <v>-32.65</v>
+        <v>-6.37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B10">
-        <v>4500</v>
+        <v>5500</v>
       </c>
       <c r="C10">
-        <v>-1.41</v>
+        <v>-8.67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -9368,65 +10408,65 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>6500</v>
+        <v>5500</v>
       </c>
       <c r="C11">
-        <v>-18.62</v>
+        <v>-9.9499999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B12">
-        <v>7500</v>
+        <v>5500</v>
       </c>
       <c r="C12">
-        <v>-27.44</v>
+        <v>-10.07</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B13">
         <v>5500</v>
       </c>
       <c r="C13">
-        <v>-9.9700000000000006</v>
+        <v>-10.65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B14">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="C14">
-        <v>-27.59</v>
+        <v>-15.27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B15">
-        <v>5500</v>
+        <v>6500</v>
       </c>
       <c r="C15">
-        <v>-10.09</v>
+        <v>-18.079999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B16">
-        <v>8035</v>
+        <v>6500</v>
       </c>
       <c r="C16">
-        <v>-32.29</v>
+        <v>-18.63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -9434,54 +10474,54 @@
         <v>64</v>
       </c>
       <c r="B17">
-        <v>4500</v>
+        <v>6500</v>
       </c>
       <c r="C17">
-        <v>-1.56</v>
+        <v>-18.68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B18">
         <v>6500</v>
       </c>
       <c r="C18">
-        <v>-18.68</v>
+        <v>-19.25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B19">
-        <v>4500</v>
+        <v>7000</v>
       </c>
       <c r="C19">
-        <v>-2.09</v>
+        <v>-24.38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B20">
-        <v>6500</v>
+        <v>7500</v>
       </c>
       <c r="C20">
-        <v>-19.260000000000002</v>
+        <v>-27.45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21">
-        <v>8047</v>
+        <v>7500</v>
       </c>
       <c r="C21">
-        <v>-33.35</v>
+        <v>-27.58</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -9489,54 +10529,54 @@
         <v>66</v>
       </c>
       <c r="B22">
-        <v>5500</v>
+        <v>7500</v>
       </c>
       <c r="C22">
-        <v>-10.68</v>
+        <v>-28.3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>7500</v>
       </c>
       <c r="C23">
-        <v>-28.29</v>
+        <v>-28.3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B24">
-        <v>7000</v>
+        <v>8035</v>
       </c>
       <c r="C24">
-        <v>-24.41</v>
+        <v>-32.299999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B25">
-        <v>6000</v>
+        <v>8068</v>
       </c>
       <c r="C25">
-        <v>-15.29</v>
+        <v>-32.67</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26">
-        <v>8612</v>
+        <v>8047</v>
       </c>
       <c r="C26">
-        <v>-39.44</v>
+        <v>-33.32</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -9544,21 +10584,21 @@
         <v>68</v>
       </c>
       <c r="B27">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="C27">
-        <v>-6.38</v>
+        <v>-33.58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B28">
-        <v>4000</v>
+        <v>8125</v>
       </c>
       <c r="C28">
-        <v>2.2599999999999998</v>
+        <v>-34.549999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -9566,10 +10606,10 @@
         <v>68</v>
       </c>
       <c r="B29">
-        <v>8000</v>
+        <v>8612</v>
       </c>
       <c r="C29">
-        <v>-33.619999999999997</v>
+        <v>-39.450000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -9580,10 +10620,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEA83A2-F7C1-45B5-ACF9-AD88CF9F080B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9613,156 +10653,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>45.832500000000003</v>
+        <v>27.988060000000001</v>
       </c>
       <c r="C2">
-        <v>-10.32</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B3">
-        <v>63.068890000000003</v>
+        <v>27.962499999999999</v>
       </c>
       <c r="C3">
-        <v>-20.78</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B4">
-        <v>36.578330000000001</v>
+        <v>27.86167</v>
       </c>
       <c r="C4">
-        <v>-1.28</v>
+        <v>9.4700000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <v>27.988060000000001</v>
+        <v>27.702220000000001</v>
       </c>
       <c r="C5">
-        <v>10.32</v>
+        <v>9.08</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B6">
-        <v>35.237200000000001</v>
+        <v>28.353059999999999</v>
       </c>
       <c r="C6">
-        <v>0.79</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B7">
-        <v>27.702220000000001</v>
+        <v>28.095829999999999</v>
       </c>
       <c r="C7">
-        <v>9.18</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B8">
-        <v>27.962499999999999</v>
+        <v>27.920829999999999</v>
       </c>
       <c r="C8">
-        <v>10.32</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B9">
-        <v>28.698060000000002</v>
+        <v>27.891940000000002</v>
       </c>
       <c r="C9">
-        <v>4.68</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B10">
-        <v>27.86167</v>
+        <v>28.551939999999998</v>
       </c>
       <c r="C10">
-        <v>9.56</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B11">
-        <v>27.920829999999999</v>
+        <v>28.613610000000001</v>
       </c>
       <c r="C11">
-        <v>6.65</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <v>28.095829999999999</v>
+        <v>28.698060000000002</v>
       </c>
       <c r="C12">
-        <v>6.74</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B13">
-        <v>28.353059999999999</v>
+        <v>35.881390000000003</v>
       </c>
       <c r="C13">
-        <v>6.94</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B14">
-        <v>28.551939999999998</v>
+        <v>35.237200000000001</v>
       </c>
       <c r="C14">
-        <v>5.29</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>28.613610000000001</v>
+        <v>36.578330000000001</v>
       </c>
       <c r="C15">
-        <v>4.88</v>
+        <v>-1.28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -9773,7 +10813,7 @@
         <v>35.724170000000001</v>
       </c>
       <c r="C16">
-        <v>-1.41</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -9784,7 +10824,7 @@
         <v>35.759169999999997</v>
       </c>
       <c r="C17">
-        <v>-1.56</v>
+        <v>-1.55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -9795,28 +10835,39 @@
         <v>35.81306</v>
       </c>
       <c r="C18">
-        <v>-2.09</v>
+        <v>-2.08</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>35.881390000000003</v>
+        <v>45.832500000000003</v>
       </c>
       <c r="C19">
-        <v>2.2599999999999998</v>
+        <v>-10.15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>63.068890000000003</v>
+      </c>
+      <c r="C20">
+        <v>-20.78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>70</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>78.633889999999994</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>-50.02</v>
       </c>
     </row>
@@ -9828,10 +10879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BE5266-FC73-4D9D-9C49-A5AB744C0DAF}">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9846,208 +10897,208 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>-0.32</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>10.29</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B3">
-        <v>-18.21</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>31.91</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B4">
-        <v>14.35</v>
+        <v>10.17</v>
       </c>
       <c r="C4">
-        <v>5.59</v>
+        <v>9.4700000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <v>7.38</v>
+        <v>9.33</v>
       </c>
       <c r="C5">
-        <v>6.03</v>
+        <v>9.08</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B6">
-        <v>-10.32</v>
+        <v>11.92</v>
       </c>
       <c r="C6">
-        <v>21.32</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B7">
-        <v>12.85</v>
+        <v>13.25</v>
       </c>
       <c r="C7">
-        <v>15.15</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B8">
-        <v>5.56</v>
+        <v>9.5</v>
       </c>
       <c r="C8">
-        <v>25.29</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B9">
-        <v>15.18</v>
+        <v>8.67</v>
       </c>
       <c r="C9">
-        <v>11.62</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B10">
-        <v>11.82</v>
+        <v>10.33</v>
       </c>
       <c r="C10">
-        <v>15.44</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B11">
-        <v>21.29</v>
+        <v>13.17</v>
       </c>
       <c r="C11">
-        <v>7.35</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <v>9.32</v>
+        <v>13.67</v>
       </c>
       <c r="C12">
-        <v>6.5</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B13">
-        <v>5.13</v>
+        <v>9.42</v>
       </c>
       <c r="C13">
-        <v>9.33</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B14">
-        <v>-11.12</v>
+        <v>8.67</v>
       </c>
       <c r="C14">
-        <v>8.75</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>5.63</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>-1.28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B16">
-        <v>-20.78</v>
+        <v>7.5</v>
       </c>
       <c r="C16">
-        <v>13.58</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B17">
-        <v>-2.12</v>
+        <v>8.33</v>
       </c>
       <c r="C17">
-        <v>5.58</v>
+        <v>-1.55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="B18">
-        <v>-30.8</v>
+        <v>10.17</v>
       </c>
       <c r="C18">
-        <v>19.75</v>
+        <v>-2.08</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>-37.65</v>
+        <v>21.83</v>
       </c>
       <c r="C19">
-        <v>23.75</v>
+        <v>-10.15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -10055,1180 +11106,26 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>12.43</v>
+        <v>13.58</v>
       </c>
       <c r="C20">
-        <v>3.42</v>
+        <v>-20.78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B21">
-        <v>-1.28</v>
+        <v>38.83</v>
       </c>
       <c r="C21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <v>7.77</v>
-      </c>
-      <c r="C22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23">
-        <v>22.93</v>
-      </c>
-      <c r="C23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>15.78</v>
-      </c>
-      <c r="C24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>-4.26</v>
-      </c>
-      <c r="C25">
-        <v>12.79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26">
-        <v>-28.09</v>
-      </c>
-      <c r="C26">
-        <v>20.29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27">
-        <v>3.29</v>
-      </c>
-      <c r="C27">
-        <v>10.29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>-20.65</v>
-      </c>
-      <c r="C28">
-        <v>17.649999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29">
-        <v>-12.18</v>
-      </c>
-      <c r="C29">
-        <v>15.15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>10.32</v>
-      </c>
-      <c r="C30">
-        <v>8.68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31">
-        <v>-8.56</v>
-      </c>
-      <c r="C31">
-        <v>11.76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32">
-        <v>-18.03</v>
-      </c>
-      <c r="C32">
-        <v>15.74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33">
-        <v>-34.5</v>
-      </c>
-      <c r="C33">
-        <v>21.62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34">
-        <v>16.53</v>
-      </c>
-      <c r="C34">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35">
-        <v>9.3800000000000008</v>
-      </c>
-      <c r="C35">
-        <v>5.44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36">
-        <v>0.79</v>
-      </c>
-      <c r="C36">
-        <v>8.82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>-28.24</v>
-      </c>
-      <c r="C37">
-        <v>19.260000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38">
-        <v>-20.47</v>
-      </c>
-      <c r="C38">
-        <v>23.97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39">
-        <v>15.47</v>
-      </c>
-      <c r="C39">
-        <v>8.09</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>9.18</v>
-      </c>
-      <c r="C40">
-        <v>9.1199999999999992</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>-5.0599999999999996</v>
-      </c>
-      <c r="C41">
-        <v>15.15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="C42">
-        <v>11.91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B43">
-        <v>-12.62</v>
-      </c>
-      <c r="C43">
-        <v>19.559999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44">
-        <v>22.24</v>
-      </c>
-      <c r="C44">
-        <v>8.09</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45">
-        <v>-25.12</v>
-      </c>
-      <c r="C45">
-        <v>26.62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46">
-        <v>-25.03</v>
-      </c>
-      <c r="C46">
-        <v>18.97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47">
-        <v>-20.62</v>
-      </c>
-      <c r="C47">
-        <v>17.350000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48">
-        <v>-4.24</v>
-      </c>
-      <c r="C48">
-        <v>12.79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49">
-        <v>10.32</v>
-      </c>
-      <c r="C49">
-        <v>8.68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50">
-        <v>3.21</v>
-      </c>
-      <c r="C50">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51">
-        <v>-12.18</v>
-      </c>
-      <c r="C51">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52">
-        <v>4.68</v>
-      </c>
-      <c r="C52">
-        <v>13.24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53">
-        <v>18.62</v>
-      </c>
-      <c r="C53">
-        <v>13.38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54">
-        <v>25.21</v>
-      </c>
-      <c r="C54">
-        <v>13.09</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>44</v>
-      </c>
-      <c r="B55">
-        <v>-18.59</v>
-      </c>
-      <c r="C55">
-        <v>19.559999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>44</v>
-      </c>
-      <c r="B56">
-        <v>-10.38</v>
-      </c>
-      <c r="C56">
-        <v>16.760000000000002</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57">
-        <v>-2.76</v>
-      </c>
-      <c r="C57">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58">
-        <v>-24</v>
-      </c>
-      <c r="C58">
-        <v>22.35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>44</v>
-      </c>
-      <c r="B59">
-        <v>11.74</v>
-      </c>
-      <c r="C59">
-        <v>13.09</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>47</v>
-      </c>
-      <c r="B60">
-        <v>2.56</v>
-      </c>
-      <c r="C60">
-        <v>11.47</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B61">
-        <v>-10.88</v>
-      </c>
-      <c r="C61">
-        <v>14.12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62">
-        <v>9.56</v>
-      </c>
-      <c r="C62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>47</v>
-      </c>
-      <c r="B63">
-        <v>-4.53</v>
-      </c>
-      <c r="C63">
-        <v>12.79</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>47</v>
-      </c>
-      <c r="B64">
-        <v>16.29</v>
-      </c>
-      <c r="C64">
-        <v>9.7100000000000009</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65">
-        <v>-23.79</v>
-      </c>
-      <c r="C65">
-        <v>19.71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B66">
-        <v>-15.74</v>
-      </c>
-      <c r="C66">
-        <v>15.88</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>49</v>
-      </c>
-      <c r="B67">
-        <v>19.18</v>
-      </c>
-      <c r="C67">
-        <v>8.3800000000000008</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>49</v>
-      </c>
-      <c r="B68">
-        <v>-8.1199999999999992</v>
-      </c>
-      <c r="C68">
-        <v>13.38</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>49</v>
-      </c>
-      <c r="B69">
-        <v>12.79</v>
-      </c>
-      <c r="C69">
-        <v>7.79</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70">
-        <v>6.18</v>
-      </c>
-      <c r="C70">
-        <v>8.5299999999999994</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>51</v>
-      </c>
-      <c r="B71">
-        <v>-0.68</v>
-      </c>
-      <c r="C71">
-        <v>11.62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72">
-        <v>6.65</v>
-      </c>
-      <c r="C72">
-        <v>9.26</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>51</v>
-      </c>
-      <c r="B73">
-        <v>-5.71</v>
-      </c>
-      <c r="C73">
-        <v>12.94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>51</v>
-      </c>
-      <c r="B74">
-        <v>13.47</v>
-      </c>
-      <c r="C74">
-        <v>8.24</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75">
-        <v>6.74</v>
-      </c>
-      <c r="C75">
-        <v>12.79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>53</v>
-      </c>
-      <c r="B76">
-        <v>-23.71</v>
-      </c>
-      <c r="C76">
-        <v>22.21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>53</v>
-      </c>
-      <c r="B77">
-        <v>-1.03</v>
-      </c>
-      <c r="C77">
-        <v>14.71</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>53</v>
-      </c>
-      <c r="B78">
-        <v>-17.559999999999999</v>
-      </c>
-      <c r="C78">
-        <v>20.149999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79">
-        <v>-9</v>
-      </c>
-      <c r="C79">
-        <v>17.21</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>55</v>
-      </c>
-      <c r="B80">
-        <v>-17.149999999999999</v>
-      </c>
-      <c r="C80">
-        <v>19.559999999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>55</v>
-      </c>
-      <c r="B81">
-        <v>6.94</v>
-      </c>
-      <c r="C81">
-        <v>11.47</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>55</v>
-      </c>
-      <c r="B82">
-        <v>-0.68</v>
-      </c>
-      <c r="C82">
-        <v>13.24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>55</v>
-      </c>
-      <c r="B83">
-        <v>-8.56</v>
-      </c>
-      <c r="C83">
-        <v>16.47</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>55</v>
-      </c>
-      <c r="B84">
-        <v>-21.79</v>
-      </c>
-      <c r="C84">
-        <v>20.88</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>57</v>
-      </c>
-      <c r="B85">
-        <v>11.79</v>
-      </c>
-      <c r="C85">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>57</v>
-      </c>
-      <c r="B86">
-        <v>-15.71</v>
-      </c>
-      <c r="C86">
-        <v>12.94</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>57</v>
-      </c>
-      <c r="B87">
-        <v>-1.56</v>
-      </c>
-      <c r="C87">
-        <v>11.03</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>57</v>
-      </c>
-      <c r="B88">
-        <v>18.18</v>
-      </c>
-      <c r="C88">
-        <v>10.29</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>57</v>
-      </c>
-      <c r="B89">
-        <v>-20.71</v>
-      </c>
-      <c r="C89">
-        <v>13.82</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>57</v>
-      </c>
-      <c r="B90">
-        <v>5.29</v>
-      </c>
-      <c r="C90">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>57</v>
-      </c>
-      <c r="B91">
-        <v>-8.4700000000000006</v>
-      </c>
-      <c r="C91">
-        <v>12.06</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>57</v>
-      </c>
-      <c r="B92">
-        <v>24.76</v>
-      </c>
-      <c r="C92">
-        <v>10.29</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>59</v>
-      </c>
-      <c r="B93">
-        <v>-21.91</v>
-      </c>
-      <c r="C93">
-        <v>17.940000000000001</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>59</v>
-      </c>
-      <c r="B94">
-        <v>11.71</v>
-      </c>
-      <c r="C94">
-        <v>11.76</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>59</v>
-      </c>
-      <c r="B95">
-        <v>18.260000000000002</v>
-      </c>
-      <c r="C95">
-        <v>11.76</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>59</v>
-      </c>
-      <c r="B96">
-        <v>-17.239999999999998</v>
-      </c>
-      <c r="C96">
-        <v>16.32</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B97">
-        <v>-9.65</v>
-      </c>
-      <c r="C97">
-        <v>15.29</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>59</v>
-      </c>
-      <c r="B98">
-        <v>-2.09</v>
-      </c>
-      <c r="C98">
-        <v>13.38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B99">
-        <v>4.88</v>
-      </c>
-      <c r="C99">
-        <v>12.79</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>61</v>
-      </c>
-      <c r="B100">
-        <v>-9.9700000000000006</v>
-      </c>
-      <c r="C100">
-        <v>9.7100000000000009</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>61</v>
-      </c>
-      <c r="B101">
-        <v>-32.65</v>
-      </c>
-      <c r="C101">
-        <v>14.26</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>61</v>
-      </c>
-      <c r="B102">
-        <v>-1.41</v>
-      </c>
-      <c r="C102">
-        <v>7.35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>61</v>
-      </c>
-      <c r="B103">
-        <v>-18.62</v>
-      </c>
-      <c r="C103">
-        <v>11.03</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>61</v>
-      </c>
-      <c r="B104">
-        <v>-27.44</v>
-      </c>
-      <c r="C104">
-        <v>12.79</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>64</v>
-      </c>
-      <c r="B105">
-        <v>-32.29</v>
-      </c>
-      <c r="C105">
-        <v>14.26</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>64</v>
-      </c>
-      <c r="B106">
-        <v>-1.56</v>
-      </c>
-      <c r="C106">
-        <v>8.24</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>64</v>
-      </c>
-      <c r="B107">
-        <v>-27.59</v>
-      </c>
-      <c r="C107">
-        <v>12.94</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>64</v>
-      </c>
-      <c r="B108">
-        <v>-10.09</v>
-      </c>
-      <c r="C108">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>64</v>
-      </c>
-      <c r="B109">
-        <v>-18.68</v>
-      </c>
-      <c r="C109">
-        <v>11.03</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>66</v>
-      </c>
-      <c r="B110">
-        <v>-2.09</v>
-      </c>
-      <c r="C110">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>66</v>
-      </c>
-      <c r="B111">
-        <v>-28.29</v>
-      </c>
-      <c r="C111">
-        <v>15.15</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>66</v>
-      </c>
-      <c r="B112">
-        <v>-10.68</v>
-      </c>
-      <c r="C112">
-        <v>10.88</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>66</v>
-      </c>
-      <c r="B113">
-        <v>-33.35</v>
-      </c>
-      <c r="C113">
-        <v>15.74</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>66</v>
-      </c>
-      <c r="B114">
-        <v>-19.260000000000002</v>
-      </c>
-      <c r="C114">
-        <v>13.68</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>68</v>
-      </c>
-      <c r="B115">
-        <v>-33.619999999999997</v>
-      </c>
-      <c r="C115">
-        <v>18.239999999999998</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>68</v>
-      </c>
-      <c r="B116">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="C116">
-        <v>9.41</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>68</v>
-      </c>
-      <c r="B117">
-        <v>-24.41</v>
-      </c>
-      <c r="C117">
-        <v>15.59</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>68</v>
-      </c>
-      <c r="B118">
-        <v>-39.44</v>
-      </c>
-      <c r="C118">
-        <v>20.29</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>68</v>
-      </c>
-      <c r="B119">
-        <v>-6.38</v>
-      </c>
-      <c r="C119">
-        <v>11.47</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>68</v>
-      </c>
-      <c r="B120">
-        <v>-15.29</v>
-      </c>
-      <c r="C120">
-        <v>13.82</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>70</v>
-      </c>
-      <c r="B121">
-        <v>-17.02</v>
-      </c>
-      <c r="C121">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>70</v>
-      </c>
-      <c r="B122">
-        <v>-59.97</v>
-      </c>
-      <c r="C122">
-        <v>54.67</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>70</v>
-      </c>
-      <c r="B123">
-        <v>-30.45</v>
-      </c>
-      <c r="C123">
-        <v>14.17</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>70</v>
-      </c>
-      <c r="B124">
         <v>-50.02</v>
-      </c>
-      <c r="C124">
-        <v>38.83</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>70</v>
-      </c>
-      <c r="B125">
-        <v>-24.88</v>
-      </c>
-      <c r="C125">
-        <v>11.58</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>70</v>
-      </c>
-      <c r="B126">
-        <v>-38.479999999999997</v>
-      </c>
-      <c r="C126">
-        <v>21.92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11236,7 +11133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CD232B-E5ED-49DF-9162-19843A25CEDF}">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>